<commit_message>
Added new tabs to the master data file
</commit_message>
<xml_diff>
--- a/TestEnvironment/MasterData/MasterDataFile.xlsx
+++ b/TestEnvironment/MasterData/MasterDataFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neeraj\PycharmProjects\MIMO\TestEnvironment\MasterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329BA48D-036C-4F5C-A18C-300398421AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA486CBB-05ED-4EF7-BFA4-317DAD71B047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalData" sheetId="2" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="test_Smoke_Administration_Admin" sheetId="8" r:id="rId7"/>
     <sheet name="test_Smoke_Home_Superintendent" sheetId="9" r:id="rId8"/>
     <sheet name="test_Smoke_Properties_Superinte" sheetId="10" r:id="rId9"/>
+    <sheet name="test_Smoke_Inspections_Superint" sheetId="11" r:id="rId10"/>
+    <sheet name="test_Smoke_WorkOrders_Superinte" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="256">
   <si>
     <t>AdminUsername</t>
   </si>
@@ -1182,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F363D98D-09C5-44C0-921A-BBB06DDB1366}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="BC11" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1377,6 +1379,362 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA81E54-4927-461F-BCC2-9BA3A9808897}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B878A8-414E-43D4-876F-1551A05A41D8}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>